<commit_message>
Bảng kế hoạch 10/10/2019
</commit_message>
<xml_diff>
--- a/BangKeHoach-DoAnCuoiKyCTDL (1).xlsx
+++ b/BangKeHoach-DoAnCuoiKyCTDL (1).xlsx
@@ -63,9 +63,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Tìm hiểu về đồ họa trong C# và đề ra mục tiêu về giao diện chương trình.</t>
-  </si>
-  <si>
     <t>Tìm hiểu về những yêu cầu của người dùng đối với chương trình cần tạo ra.</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Nhìn nhận những ưu nhược điểm của chương trình đã tạo ra và đề ra hướng khắc phục cho những đồ án sau này.</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về đồ họa trong C++ và đề ra mục tiêu về giao diện chương trình.</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -769,7 +769,7 @@
     </row>
     <row r="6" spans="1:23" s="16" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="16" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>12</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="7" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>12</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="8" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20" t="s">
@@ -879,7 +879,7 @@
     </row>
     <row r="9" spans="1:23" s="16" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
@@ -905,7 +905,7 @@
     </row>
     <row r="10" spans="1:23" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>12</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="11" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -969,7 +969,7 @@
     </row>
     <row r="12" spans="1:23" s="16" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -995,7 +995,7 @@
     </row>
     <row r="13" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20" t="s">
@@ -1031,7 +1031,7 @@
     </row>
     <row r="14" spans="1:23" s="16" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>12</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="15" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="16" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>12</v>
@@ -1104,10 +1104,10 @@
         <v>43753</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="7">
-        <v>43770</v>
+        <v>43739</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="8"/>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="17" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
@@ -1138,10 +1138,10 @@
         <v>43753</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" s="7">
-        <v>43770</v>
+        <v>43739</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="8"/>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="18" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>12</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="19" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>12</v>
@@ -1230,10 +1230,10 @@
     </row>
     <row r="20" spans="1:23" s="16" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>12</v>

</xml_diff>